<commit_message>
fixing 2016 and working through - much cleaner yay!
</commit_message>
<xml_diff>
--- a/2016/Cameras_2016_work.xlsx
+++ b/2016/Cameras_2016_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96380853-D67F-8341-A291-D6D7F88616E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FE3751-F8FD-6341-87C8-74A3FC6FA6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16000" xr2:uid="{03E0F979-A2DD-0344-9B4A-9D4630B07C3F}"/>
   </bookViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,7 +721,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="6">
-        <v>42013</v>
+        <v>42378</v>
       </c>
       <c r="D2" s="7">
         <v>42481</v>
@@ -774,7 +774,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="6">
-        <v>42013</v>
+        <v>42378</v>
       </c>
       <c r="D3" s="7">
         <v>42481</v>
@@ -827,7 +827,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="6">
-        <v>42013</v>
+        <v>42378</v>
       </c>
       <c r="D4" s="7">
         <v>42481</v>
@@ -880,7 +880,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="6">
-        <v>42013</v>
+        <v>42378</v>
       </c>
       <c r="D5" s="7">
         <v>42481</v>
@@ -933,7 +933,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="6">
-        <v>42013</v>
+        <v>42378</v>
       </c>
       <c r="D6" s="7">
         <v>42481</v>
@@ -986,7 +986,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="6">
-        <v>42013</v>
+        <v>42378</v>
       </c>
       <c r="D7" s="7">
         <v>42481</v>

</xml_diff>